<commit_message>
aanpassing met aantallen voor fluit en zaaldienst
</commit_message>
<xml_diff>
--- a/Thuiswedstrijden.xlsx
+++ b/Thuiswedstrijden.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\github\volleybalwedstrijdschema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5A5FD7A-2D9D-4716-A35D-B4328031F2EA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B653B9-2ADB-4EF3-84EC-CEA7226C39FF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Wedstrijden" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Wedstrijden!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Wedstrijden!$A$1:$G$233</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="185">
   <si>
     <t>Datum</t>
   </si>
@@ -536,6 +536,48 @@
   </si>
   <si>
     <t>Sporthal Schalkhaar, SCHALKHAAR</t>
+  </si>
+  <si>
+    <t>Scheidsrechters van team</t>
+  </si>
+  <si>
+    <t>Zaaldienst</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>BOND</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>MA2</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>MA1</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Henk Cordes</t>
+  </si>
+  <si>
+    <t>Alouis (onv Keppels)</t>
   </si>
 </sst>
 </file>
@@ -545,7 +587,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -557,13 +599,25 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -575,16 +629,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -887,11 +946,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E233"/>
+  <dimension ref="A1:G233"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,9 +958,11 @@
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -917,8 +978,14 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>5</v>
       </c>
@@ -929,18 +996,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43726</v>
       </c>
@@ -957,41 +1028,53 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>43728</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="6">
         <v>43728.791666666999</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="F5" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>43728</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="6">
         <v>43728.791666666999</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43728</v>
       </c>
@@ -1008,24 +1091,30 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>43728</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="6">
         <v>43728.875</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43728</v>
       </c>
@@ -1042,24 +1131,30 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
         <v>43728</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="6">
         <v>43728.875</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43729</v>
       </c>
@@ -1076,7 +1171,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43729</v>
       </c>
@@ -1093,7 +1188,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43729</v>
       </c>
@@ -1110,41 +1205,53 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
         <v>43735</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="6">
         <v>43735.854166666999</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="F14" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
         <v>43735</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="6">
         <v>43735.854166666999</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43735</v>
       </c>
@@ -1161,7 +1268,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43735</v>
       </c>
@@ -1178,75 +1285,99 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <v>43736</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="6">
         <v>43736.541666666999</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="F18" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
         <v>43736</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="6">
         <v>43736.541666666999</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="F19" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
         <v>43736</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="6">
         <v>43736.625</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="F20" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
         <v>43736</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="6">
         <v>43736.625</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43736</v>
       </c>
@@ -1263,7 +1394,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43736</v>
       </c>
@@ -1280,24 +1411,30 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
         <v>43736</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="6">
         <v>43736.708333333001</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43740</v>
       </c>
@@ -1314,7 +1451,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43740</v>
       </c>
@@ -1331,24 +1468,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
         <v>43742</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="6">
         <v>43742.791666666999</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43742</v>
       </c>
@@ -1365,24 +1508,30 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
         <v>43742</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="6">
         <v>43742.875</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43742</v>
       </c>
@@ -1399,24 +1548,30 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
         <v>43742</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="6">
         <v>43742.875</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43743</v>
       </c>
@@ -1433,7 +1588,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43743</v>
       </c>
@@ -1450,7 +1605,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43743</v>
       </c>
@@ -1467,7 +1622,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43743</v>
       </c>
@@ -1484,7 +1639,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43746</v>
       </c>
@@ -1501,7 +1656,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43747</v>
       </c>
@@ -1518,7 +1673,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43747</v>
       </c>
@@ -1535,7 +1690,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43747</v>
       </c>
@@ -1552,7 +1707,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43747</v>
       </c>
@@ -1569,7 +1724,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43749</v>
       </c>
@@ -1586,7 +1741,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43749</v>
       </c>
@@ -1603,7 +1758,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43749</v>
       </c>
@@ -1620,109 +1775,145 @@
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
         <v>43749</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="6">
         <v>43749.854166666999</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+      <c r="F44" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
         <v>43749</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="6">
         <v>43749.854166666999</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+      <c r="F45" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
         <v>43750</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="6">
         <v>43750.541666666999</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
+      <c r="F46" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
         <v>43750</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="6">
         <v>43750.541666666999</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+      <c r="F47" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
         <v>43750</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="6">
         <v>43750.625</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+      <c r="F48" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
         <v>43750</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="6">
         <v>43750.625</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43750</v>
       </c>
@@ -1739,24 +1930,30 @@
         <v>67</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="5">
         <v>43750</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="6">
         <v>43750.708333333001</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43754</v>
       </c>
@@ -1773,7 +1970,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43755</v>
       </c>
@@ -1790,7 +1987,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>43755</v>
       </c>
@@ -1807,41 +2004,53 @@
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="5">
         <v>43756</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="6">
         <v>43756.791666666999</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
+      <c r="F55" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="5">
         <v>43756</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="6">
         <v>43756.791666666999</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43756</v>
       </c>
@@ -1858,24 +2067,30 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="5">
         <v>43756</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="6">
         <v>43756.875</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43756</v>
       </c>
@@ -1892,24 +2107,30 @@
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="5">
         <v>43756</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="6">
         <v>43756.875</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43756</v>
       </c>
@@ -1926,24 +2147,30 @@
         <v>95</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="5">
         <v>43757</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="6">
         <v>43757.541666666999</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>43757</v>
       </c>
@@ -1960,7 +2187,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43763</v>
       </c>
@@ -1977,7 +2204,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>43764</v>
       </c>
@@ -1994,7 +2221,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>43764</v>
       </c>
@@ -2011,7 +2238,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>43769</v>
       </c>
@@ -2028,7 +2255,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>43770</v>
       </c>
@@ -2045,7 +2272,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>43770</v>
       </c>
@@ -2062,41 +2289,53 @@
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="5">
         <v>43770</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70" s="6">
         <v>43770.854166666999</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
+      <c r="F70" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="5">
         <v>43770</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71" s="6">
         <v>43770.854166666999</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>43770</v>
       </c>
@@ -2113,7 +2352,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>43771</v>
       </c>
@@ -2130,109 +2369,145 @@
         <v>112</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="5">
         <v>43771</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74" s="6">
         <v>43771.479166666999</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
+      <c r="F74" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="5">
         <v>43771</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75" s="6">
         <v>43771.479166666999</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
+      <c r="F75" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="5">
         <v>43771</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76" s="6">
         <v>43771.75</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
+      <c r="F76" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="5">
         <v>43771</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B77" s="6">
         <v>43771.75</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
+      <c r="F77" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="5">
         <v>43777</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B78" s="6">
         <v>43777.791666666999</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
+      <c r="F78" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="5">
         <v>43777</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B79" s="6">
         <v>43777.791666666999</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>43777</v>
       </c>
@@ -2249,41 +2524,53 @@
         <v>116</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="5">
         <v>43777</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B81" s="6">
         <v>43777.875</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
+      <c r="F81" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="5">
         <v>43777</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B82" s="6">
         <v>43777.875</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D82" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>43777</v>
       </c>
@@ -2300,7 +2587,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>43778</v>
       </c>
@@ -2317,7 +2604,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>43778</v>
       </c>
@@ -2334,7 +2621,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>43778</v>
       </c>
@@ -2351,7 +2638,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>43784</v>
       </c>
@@ -2368,7 +2655,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>43784</v>
       </c>
@@ -2385,75 +2672,99 @@
         <v>124</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="5">
         <v>43784</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B89" s="6">
         <v>43784.854166666999</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E89" t="s">
+      <c r="E89" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
+      <c r="F89" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="5">
         <v>43784</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B90" s="6">
         <v>43784.854166666999</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E90" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
+      <c r="F90" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="5">
         <v>43785</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B91" s="6">
         <v>43785.479166666999</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E91" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
+      <c r="F91" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="5">
         <v>43785</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B92" s="6">
         <v>43785.479166666999</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E92" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F92" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>43785</v>
       </c>
@@ -2470,58 +2781,76 @@
         <v>104</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="5">
         <v>43785</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B94" s="6">
         <v>43785.572916666999</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E94" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
+      <c r="F94" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="5">
         <v>43785</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B95" s="6">
         <v>43785.572916666999</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E95" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
+      <c r="F95" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G95" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="5">
         <v>43785</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B96" s="6">
         <v>43785.666666666999</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E96" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F96" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>43789</v>
       </c>
@@ -2538,7 +2867,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>43789</v>
       </c>
@@ -2555,7 +2884,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>43790</v>
       </c>
@@ -2572,7 +2901,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>43790</v>
       </c>
@@ -2589,24 +2918,30 @@
         <v>85</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="5">
         <v>43791</v>
       </c>
-      <c r="B101" s="2">
+      <c r="B101" s="6">
         <v>43791.791666666999</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E101" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F101" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G101" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>43792</v>
       </c>
@@ -2623,7 +2958,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>43792</v>
       </c>
@@ -2640,24 +2975,30 @@
         <v>135</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="5">
         <v>43792</v>
       </c>
-      <c r="B104" s="2">
+      <c r="B104" s="6">
         <v>43792.625</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E104" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F104" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G104" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>43796</v>
       </c>
@@ -2674,7 +3015,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>43796</v>
       </c>
@@ -2691,7 +3032,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>43798</v>
       </c>
@@ -2708,109 +3049,145 @@
         <v>25</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="5">
         <v>43798</v>
       </c>
-      <c r="B108" s="2">
+      <c r="B108" s="6">
         <v>43798.854166666999</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E108" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
+      <c r="F108" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="G108" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="5">
         <v>43798</v>
       </c>
-      <c r="B109" s="2">
+      <c r="B109" s="6">
         <v>43798.854166666999</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E109" t="s">
+      <c r="E109" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
+      <c r="F109" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G109" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="5">
         <v>43798</v>
       </c>
-      <c r="B110" s="2">
+      <c r="B110" s="6">
         <v>43798.875</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E110" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
+      <c r="F110" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G110" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="5">
         <v>43798</v>
       </c>
-      <c r="B111" s="2">
+      <c r="B111" s="6">
         <v>43798.875</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E111" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
+      <c r="F111" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G111" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="5">
         <v>43799</v>
       </c>
-      <c r="B112" s="2">
+      <c r="B112" s="6">
         <v>43799.541666666999</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C112" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="E112" t="s">
+      <c r="E112" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
+      <c r="F112" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G112" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="5">
         <v>43799</v>
       </c>
-      <c r="B113" s="2">
+      <c r="B113" s="6">
         <v>43799.541666666999</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E113" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F113" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G113" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>43799</v>
       </c>
@@ -2827,7 +3204,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>43799</v>
       </c>
@@ -2844,24 +3221,30 @@
         <v>104</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="1">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="5">
         <v>43799</v>
       </c>
-      <c r="B116" s="2">
+      <c r="B116" s="6">
         <v>43799.625</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D116" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E116" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F116" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G116" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>43803</v>
       </c>
@@ -2878,7 +3261,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>43803</v>
       </c>
@@ -2895,24 +3278,30 @@
         <v>144</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="1">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="5">
         <v>43805</v>
       </c>
-      <c r="B119" s="2">
+      <c r="B119" s="6">
         <v>43805.791666666999</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C119" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D119" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E119" t="s">
+      <c r="E119" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F119" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G119" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>43805</v>
       </c>
@@ -2929,7 +3318,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>43805</v>
       </c>
@@ -2946,7 +3335,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>43805</v>
       </c>
@@ -2963,7 +3352,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>43805</v>
       </c>
@@ -2980,7 +3369,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>43810</v>
       </c>
@@ -2997,7 +3386,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>43810</v>
       </c>
@@ -3014,7 +3403,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>43812</v>
       </c>
@@ -3031,41 +3420,53 @@
         <v>76</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="1">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="5">
         <v>43812</v>
       </c>
-      <c r="B127" s="2">
+      <c r="B127" s="6">
         <v>43812.854166666999</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C127" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D127" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E127" t="s">
+      <c r="E127" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" s="1">
+      <c r="F127" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G127" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="5">
         <v>43812</v>
       </c>
-      <c r="B128" s="2">
+      <c r="B128" s="6">
         <v>43812.854166666999</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C128" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D128" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="E128" t="s">
+      <c r="E128" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F128" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G128" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>43812</v>
       </c>
@@ -3082,7 +3483,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>43813</v>
       </c>
@@ -3099,7 +3500,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>43813</v>
       </c>
@@ -3116,7 +3517,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>43813</v>
       </c>
@@ -3133,24 +3534,30 @@
         <v>154</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="1">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" s="5">
         <v>43813</v>
       </c>
-      <c r="B133" s="2">
+      <c r="B133" s="6">
         <v>43813.708333333001</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C133" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D133" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="E133" t="s">
+      <c r="E133" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F133" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G133" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>43813</v>
       </c>
@@ -3167,7 +3574,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>43813</v>
       </c>
@@ -3184,7 +3591,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>43817</v>
       </c>
@@ -3201,7 +3608,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>43817</v>
       </c>
@@ -3218,7 +3625,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>43819</v>
       </c>
@@ -3235,7 +3642,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>43839</v>
       </c>
@@ -3252,7 +3659,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>43839</v>
       </c>
@@ -3269,7 +3676,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>43839</v>
       </c>
@@ -3286,7 +3693,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>43839</v>
       </c>
@@ -3303,58 +3710,70 @@
         <v>104</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" s="1">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" s="5">
         <v>43840</v>
       </c>
-      <c r="B143" s="2">
+      <c r="B143" s="6">
         <v>43840.791666666999</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C143" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D143" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E143" t="s">
+      <c r="E143" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A144" s="1">
+      <c r="F143" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G143" s="4"/>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="5">
         <v>43840</v>
       </c>
-      <c r="B144" s="2">
+      <c r="B144" s="6">
         <v>43840.791666666999</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C144" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D144" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E144" t="s">
+      <c r="E144" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" s="1">
+      <c r="F144" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G144" s="4"/>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="5">
         <v>43840</v>
       </c>
-      <c r="B145" s="2">
+      <c r="B145" s="6">
         <v>43840.875</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C145" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D145" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E145" t="s">
+      <c r="E145" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F145" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G145" s="4"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>43840</v>
       </c>
@@ -3371,24 +3790,28 @@
         <v>159</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A147" s="1">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" s="5">
         <v>43840</v>
       </c>
-      <c r="B147" s="2">
+      <c r="B147" s="6">
         <v>43840.875</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C147" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D147" t="s">
+      <c r="D147" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E147" t="s">
+      <c r="E147" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F147" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G147" s="4"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>43841</v>
       </c>
@@ -3405,7 +3828,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>43846</v>
       </c>
@@ -3422,41 +3845,49 @@
         <v>104</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A150" s="1">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" s="5">
         <v>43847</v>
       </c>
-      <c r="B150" s="2">
+      <c r="B150" s="6">
         <v>43847.854166666999</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C150" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D150" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E150" t="s">
+      <c r="E150" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" s="1">
+      <c r="F150" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G150" s="4"/>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" s="5">
         <v>43847</v>
       </c>
-      <c r="B151" s="2">
+      <c r="B151" s="6">
         <v>43847.854166666999</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C151" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D151" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E151" t="s">
+      <c r="E151" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F151" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G151" s="4"/>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>43848</v>
       </c>
@@ -3473,7 +3904,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>43848</v>
       </c>
@@ -3490,7 +3921,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>43848</v>
       </c>
@@ -3507,24 +3938,28 @@
         <v>160</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" s="1">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" s="5">
         <v>43848</v>
       </c>
-      <c r="B155" s="2">
+      <c r="B155" s="6">
         <v>43848.708333333001</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C155" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D155" t="s">
+      <c r="D155" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E155" t="s">
+      <c r="E155" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F155" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G155" s="4"/>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>43850</v>
       </c>
@@ -3541,7 +3976,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>43851</v>
       </c>
@@ -3558,41 +3993,49 @@
         <v>161</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A158" s="1">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" s="5">
         <v>43854</v>
       </c>
-      <c r="B158" s="2">
+      <c r="B158" s="6">
         <v>43854.791666666999</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C158" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D158" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E158" t="s">
+      <c r="E158" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A159" s="1">
+      <c r="F158" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G158" s="4"/>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159" s="5">
         <v>43854</v>
       </c>
-      <c r="B159" s="2">
+      <c r="B159" s="6">
         <v>43854.791666666999</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C159" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D159" t="s">
+      <c r="D159" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E159" t="s">
+      <c r="E159" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F159" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G159" s="4"/>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>43854</v>
       </c>
@@ -3609,41 +4052,49 @@
         <v>135</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A161" s="1">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" s="5">
         <v>43854</v>
       </c>
-      <c r="B161" s="2">
+      <c r="B161" s="6">
         <v>43854.875</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C161" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D161" t="s">
+      <c r="D161" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E161" t="s">
+      <c r="E161" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" s="1">
+      <c r="F161" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G161" s="4"/>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162" s="5">
         <v>43854</v>
       </c>
-      <c r="B162" s="2">
+      <c r="B162" s="6">
         <v>43854.875</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C162" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D162" t="s">
+      <c r="D162" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E162" t="s">
+      <c r="E162" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F162" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G162" s="4"/>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>43861</v>
       </c>
@@ -3660,41 +4111,49 @@
         <v>16</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A164" s="1">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164" s="5">
         <v>43861</v>
       </c>
-      <c r="B164" s="2">
+      <c r="B164" s="6">
         <v>43861.854166666999</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C164" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D164" t="s">
+      <c r="D164" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E164" t="s">
+      <c r="E164" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" s="1">
+      <c r="F164" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G164" s="4"/>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" s="5">
         <v>43861</v>
       </c>
-      <c r="B165" s="2">
+      <c r="B165" s="6">
         <v>43861.854166666999</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C165" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D165" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F165" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G165" s="4"/>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>43861</v>
       </c>
@@ -3711,7 +4170,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>43861</v>
       </c>
@@ -3728,7 +4187,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>43862</v>
       </c>
@@ -3745,24 +4204,28 @@
         <v>134</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A169" s="1">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A169" s="5">
         <v>43862</v>
       </c>
-      <c r="B169" s="2">
+      <c r="B169" s="6">
         <v>43862.708333333001</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C169" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F169" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G169" s="4"/>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>43866</v>
       </c>
@@ -3779,7 +4242,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>43866</v>
       </c>
@@ -3796,7 +4259,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>43866</v>
       </c>
@@ -3813,7 +4276,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>43866</v>
       </c>
@@ -3830,41 +4293,49 @@
         <v>67</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A174" s="1">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174" s="5">
         <v>43868</v>
       </c>
-      <c r="B174" s="2">
+      <c r="B174" s="6">
         <v>43868.791666666999</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C174" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D174" t="s">
+      <c r="D174" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E174" t="s">
+      <c r="E174" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" s="1">
+      <c r="F174" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="G174" s="4"/>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A175" s="5">
         <v>43868</v>
       </c>
-      <c r="B175" s="2">
+      <c r="B175" s="6">
         <v>43868.791666666999</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C175" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D175" t="s">
+      <c r="D175" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E175" t="s">
+      <c r="E175" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F175" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G175" s="4"/>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>43868</v>
       </c>
@@ -3881,7 +4352,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>43868</v>
       </c>
@@ -3898,24 +4369,28 @@
         <v>164</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A178" s="1">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178" s="5">
         <v>43868</v>
       </c>
-      <c r="B178" s="2">
+      <c r="B178" s="6">
         <v>43868.875</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C178" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E178" t="s">
+      <c r="E178" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F178" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G178" s="4"/>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>43868</v>
       </c>
@@ -3932,24 +4407,28 @@
         <v>25</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A180" s="1">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A180" s="5">
         <v>43868</v>
       </c>
-      <c r="B180" s="2">
+      <c r="B180" s="6">
         <v>43868.875</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C180" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D180" t="s">
+      <c r="D180" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E180" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F180" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G180" s="4"/>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>43876</v>
       </c>
@@ -3966,58 +4445,70 @@
         <v>134</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A182" s="1">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A182" s="5">
         <v>43876</v>
       </c>
-      <c r="B182" s="2">
+      <c r="B182" s="6">
         <v>43876.708333333001</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C182" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D182" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E182" t="s">
+      <c r="E182" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" s="1">
+      <c r="F182" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G182" s="4"/>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" s="5">
         <v>43896</v>
       </c>
-      <c r="B183" s="2">
+      <c r="B183" s="6">
         <v>43896.854166666999</v>
       </c>
-      <c r="C183" t="s">
+      <c r="C183" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E183" t="s">
+      <c r="E183" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A184" s="1">
+      <c r="F183" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="G183" s="4"/>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184" s="5">
         <v>43896</v>
       </c>
-      <c r="B184" s="2">
+      <c r="B184" s="6">
         <v>43896.854166666999</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C184" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F184" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G184" s="4"/>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>43896</v>
       </c>
@@ -4034,7 +4525,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>43896</v>
       </c>
@@ -4051,7 +4542,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>43896</v>
       </c>
@@ -4068,7 +4559,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>43897</v>
       </c>
@@ -4085,24 +4576,28 @@
         <v>112</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A189" s="1">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A189" s="5">
         <v>43897</v>
       </c>
-      <c r="B189" s="2">
+      <c r="B189" s="6">
         <v>43897.708333333001</v>
       </c>
-      <c r="C189" t="s">
+      <c r="C189" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D189" t="s">
+      <c r="D189" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E189" t="s">
+      <c r="E189" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F189" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G189" s="4"/>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>43902</v>
       </c>
@@ -4119,7 +4614,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>43902</v>
       </c>
@@ -4136,24 +4631,28 @@
         <v>104</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A192" s="1">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A192" s="5">
         <v>43903</v>
       </c>
-      <c r="B192" s="2">
+      <c r="B192" s="6">
         <v>43903.791666666999</v>
       </c>
-      <c r="C192" t="s">
+      <c r="C192" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D192" t="s">
+      <c r="D192" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E192" t="s">
+      <c r="E192" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F192" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G192" s="4"/>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>43903</v>
       </c>
@@ -4170,41 +4669,49 @@
         <v>58</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A194" s="1">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A194" s="5">
         <v>43903</v>
       </c>
-      <c r="B194" s="2">
+      <c r="B194" s="6">
         <v>43903.875</v>
       </c>
-      <c r="C194" t="s">
+      <c r="C194" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D194" t="s">
+      <c r="D194" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E194" t="s">
+      <c r="E194" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A195" s="1">
+      <c r="F194" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G194" s="4"/>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A195" s="5">
         <v>43903</v>
       </c>
-      <c r="B195" s="2">
+      <c r="B195" s="6">
         <v>43903.875</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C195" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D195" t="s">
+      <c r="D195" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E195" t="s">
+      <c r="E195" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F195" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G195" s="4"/>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>43908</v>
       </c>
@@ -4221,7 +4728,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>43908</v>
       </c>
@@ -4238,41 +4745,49 @@
         <v>13</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A198" s="1">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A198" s="5">
         <v>43910</v>
       </c>
-      <c r="B198" s="2">
+      <c r="B198" s="6">
         <v>43910.854166666999</v>
       </c>
-      <c r="C198" t="s">
+      <c r="C198" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D198" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E198" t="s">
+      <c r="E198" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A199" s="1">
+      <c r="F198" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G198" s="4"/>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A199" s="5">
         <v>43910</v>
       </c>
-      <c r="B199" s="2">
+      <c r="B199" s="6">
         <v>43910.854166666999</v>
       </c>
-      <c r="C199" t="s">
+      <c r="C199" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D199" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E199" t="s">
+      <c r="E199" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F199" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G199" s="4"/>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>43910</v>
       </c>
@@ -4289,7 +4804,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>43911</v>
       </c>
@@ -4306,7 +4821,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>43911</v>
       </c>
@@ -4323,7 +4838,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>43911</v>
       </c>
@@ -4340,7 +4855,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>43915</v>
       </c>
@@ -4357,7 +4872,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>43915</v>
       </c>
@@ -4374,7 +4889,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>43915</v>
       </c>
@@ -4391,7 +4906,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>43915</v>
       </c>
@@ -4408,92 +4923,112 @@
         <v>67</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A208" s="1">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A208" s="5">
         <v>43917</v>
       </c>
-      <c r="B208" s="2">
+      <c r="B208" s="6">
         <v>43917.791666666999</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C208" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D208" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="E208" t="s">
+      <c r="E208" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A209" s="1">
+      <c r="F208" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="G208" s="4"/>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A209" s="5">
         <v>43917</v>
       </c>
-      <c r="B209" s="2">
+      <c r="B209" s="6">
         <v>43917.854166666999</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C209" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D209" t="s">
+      <c r="D209" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="E209" t="s">
+      <c r="E209" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A210" s="1">
+      <c r="F209" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="G209" s="4"/>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A210" s="5">
         <v>43917</v>
       </c>
-      <c r="B210" s="2">
+      <c r="B210" s="6">
         <v>43917.854166666999</v>
       </c>
-      <c r="C210" t="s">
+      <c r="C210" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D210" t="s">
+      <c r="D210" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="E210" t="s">
+      <c r="E210" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A211" s="1">
+      <c r="F210" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G210" s="4"/>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A211" s="5">
         <v>43917</v>
       </c>
-      <c r="B211" s="2">
+      <c r="B211" s="6">
         <v>43917.875</v>
       </c>
-      <c r="C211" t="s">
+      <c r="C211" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D211" t="s">
+      <c r="D211" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E211" t="s">
+      <c r="E211" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A212" s="1">
+      <c r="F211" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G211" s="4"/>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A212" s="5">
         <v>43917</v>
       </c>
-      <c r="B212" s="2">
+      <c r="B212" s="6">
         <v>43917.875</v>
       </c>
-      <c r="C212" t="s">
+      <c r="C212" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D212" t="s">
+      <c r="D212" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="E212" t="s">
+      <c r="E212" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F212" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G212" s="4"/>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>43917</v>
       </c>
@@ -4510,7 +5045,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>43918</v>
       </c>
@@ -4527,58 +5062,70 @@
         <v>154</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A215" s="1">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A215" s="5">
         <v>43924</v>
       </c>
-      <c r="B215" s="2">
+      <c r="B215" s="6">
         <v>43924.791666666999</v>
       </c>
-      <c r="C215" t="s">
+      <c r="C215" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D215" t="s">
+      <c r="D215" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E215" t="s">
+      <c r="E215" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A216" s="1">
+      <c r="F215" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G215" s="4"/>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A216" s="5">
         <v>43924</v>
       </c>
-      <c r="B216" s="2">
+      <c r="B216" s="6">
         <v>43924.791666666999</v>
       </c>
-      <c r="C216" t="s">
+      <c r="C216" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D216" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="E216" t="s">
+      <c r="E216" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A217" s="1">
+      <c r="F216" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G216" s="4"/>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A217" s="5">
         <v>43924</v>
       </c>
-      <c r="B217" s="2">
+      <c r="B217" s="6">
         <v>43924.875</v>
       </c>
-      <c r="C217" t="s">
+      <c r="C217" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D217" t="s">
+      <c r="D217" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E217" t="s">
+      <c r="E217" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F217" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G217" s="4"/>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>43924</v>
       </c>
@@ -4595,24 +5142,28 @@
         <v>25</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A219" s="1">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A219" s="5">
         <v>43924</v>
       </c>
-      <c r="B219" s="2">
+      <c r="B219" s="6">
         <v>43924.875</v>
       </c>
-      <c r="C219" t="s">
+      <c r="C219" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D219" t="s">
+      <c r="D219" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="E219" t="s">
+      <c r="E219" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F219" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G219" s="4"/>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>43924</v>
       </c>
@@ -4629,7 +5180,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>43925</v>
       </c>
@@ -4646,7 +5197,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>43929</v>
       </c>
@@ -4663,7 +5214,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>43930</v>
       </c>
@@ -4680,7 +5231,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>43930</v>
       </c>
@@ -4697,7 +5248,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>43937</v>
       </c>
@@ -4714,7 +5265,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>43937</v>
       </c>
@@ -4731,7 +5282,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>43938</v>
       </c>
@@ -4748,41 +5299,49 @@
         <v>95</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A228" s="1">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A228" s="5">
         <v>43938</v>
       </c>
-      <c r="B228" s="2">
+      <c r="B228" s="6">
         <v>43938.854166666999</v>
       </c>
-      <c r="C228" t="s">
+      <c r="C228" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D228" t="s">
+      <c r="D228" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E228" t="s">
+      <c r="E228" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A229" s="1">
+      <c r="F228" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G228" s="4"/>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A229" s="5">
         <v>43938</v>
       </c>
-      <c r="B229" s="2">
+      <c r="B229" s="6">
         <v>43938.854166666999</v>
       </c>
-      <c r="C229" t="s">
+      <c r="C229" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D229" t="s">
+      <c r="D229" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E229" t="s">
+      <c r="E229" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F229" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G229" s="4"/>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>43938</v>
       </c>
@@ -4799,7 +5358,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>43939</v>
       </c>
@@ -4816,7 +5375,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>43939</v>
       </c>
@@ -4833,26 +5392,30 @@
         <v>48</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A233" s="1">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A233" s="5">
         <v>43939</v>
       </c>
-      <c r="B233" s="2">
+      <c r="B233" s="6">
         <v>43939.708333333001</v>
       </c>
-      <c r="C233" t="s">
+      <c r="C233" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D233" t="s">
+      <c r="D233" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="E233" t="s">
+      <c r="E233" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="F233" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="G233" s="4"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <autoFilter ref="A1:E1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G233" xr:uid="{47F88E0C-9F17-4727-BABF-EEEB9EA2FD37}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
heren 2 moest 2wedstrijden fluiten tijdens hun eigen uitwedstrijd
</commit_message>
<xml_diff>
--- a/Thuiswedstrijden.xlsx
+++ b/Thuiswedstrijden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\github\volleybalwedstrijdschema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B653B9-2ADB-4EF3-84EC-CEA7226C39FF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B883C1-8FF3-4634-9D8A-F49C661CE8B4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,11 +19,18 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Wedstrijden!$A$1:$G$233</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="193">
   <si>
     <t>Datum</t>
   </si>
@@ -578,6 +585,30 @@
   </si>
   <si>
     <t>Alouis (onv Keppels)</t>
+  </si>
+  <si>
+    <t>Alouis</t>
+  </si>
+  <si>
+    <t>Henk</t>
+  </si>
+  <si>
+    <t>D1*</t>
+  </si>
+  <si>
+    <t>H1*</t>
+  </si>
+  <si>
+    <t>D3*</t>
+  </si>
+  <si>
+    <t>H2*</t>
+  </si>
+  <si>
+    <t>D2*</t>
+  </si>
+  <si>
+    <t>D4*</t>
   </si>
 </sst>
 </file>
@@ -946,11 +977,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G233"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,7 +1017,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>5</v>
       </c>
@@ -1011,7 +1043,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43726</v>
       </c>
@@ -1071,10 +1103,10 @@
         <v>176</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43728</v>
       </c>
@@ -1114,7 +1146,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43728</v>
       </c>
@@ -1151,10 +1183,10 @@
         <v>175</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43729</v>
       </c>
@@ -1171,7 +1203,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43729</v>
       </c>
@@ -1188,7 +1220,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43729</v>
       </c>
@@ -1248,10 +1280,10 @@
         <v>183</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43735</v>
       </c>
@@ -1268,7 +1300,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43735</v>
       </c>
@@ -1328,7 +1360,7 @@
         <v>178</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1374,10 +1406,10 @@
         <v>180</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43736</v>
       </c>
@@ -1394,7 +1426,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43736</v>
       </c>
@@ -1434,7 +1466,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43740</v>
       </c>
@@ -1451,7 +1483,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43740</v>
       </c>
@@ -1491,7 +1523,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43742</v>
       </c>
@@ -1531,7 +1563,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43742</v>
       </c>
@@ -1568,10 +1600,10 @@
         <v>175</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43743</v>
       </c>
@@ -1588,7 +1620,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43743</v>
       </c>
@@ -1605,7 +1637,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43743</v>
       </c>
@@ -1622,7 +1654,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43743</v>
       </c>
@@ -1639,7 +1671,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43746</v>
       </c>
@@ -1656,7 +1688,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43747</v>
       </c>
@@ -1673,7 +1705,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43747</v>
       </c>
@@ -1690,7 +1722,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43747</v>
       </c>
@@ -1707,7 +1739,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43747</v>
       </c>
@@ -1724,7 +1756,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43749</v>
       </c>
@@ -1741,7 +1773,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43749</v>
       </c>
@@ -1758,7 +1790,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43749</v>
       </c>
@@ -1818,7 +1850,7 @@
         <v>183</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1864,7 +1896,7 @@
         <v>181</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -1887,7 +1919,7 @@
         <v>181</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -1910,10 +1942,10 @@
         <v>180</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43750</v>
       </c>
@@ -1953,7 +1985,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43754</v>
       </c>
@@ -1970,7 +2002,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43755</v>
       </c>
@@ -1987,7 +2019,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>43755</v>
       </c>
@@ -2047,10 +2079,10 @@
         <v>178</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43756</v>
       </c>
@@ -2087,10 +2119,10 @@
         <v>181</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43756</v>
       </c>
@@ -2127,10 +2159,10 @@
         <v>175</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43756</v>
       </c>
@@ -2170,7 +2202,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>43757</v>
       </c>
@@ -2187,7 +2219,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43763</v>
       </c>
@@ -2204,7 +2236,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>43764</v>
       </c>
@@ -2221,7 +2253,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>43764</v>
       </c>
@@ -2238,7 +2270,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>43769</v>
       </c>
@@ -2255,7 +2287,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>43770</v>
       </c>
@@ -2272,7 +2304,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>43770</v>
       </c>
@@ -2332,10 +2364,10 @@
         <v>183</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>43770</v>
       </c>
@@ -2352,7 +2384,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>43771</v>
       </c>
@@ -2409,7 +2441,7 @@
         <v>16</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>182</v>
@@ -2435,7 +2467,7 @@
         <v>179</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2504,10 +2536,10 @@
         <v>173</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>43777</v>
       </c>
@@ -2567,10 +2599,10 @@
         <v>175</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>43777</v>
       </c>
@@ -2587,7 +2619,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>43778</v>
       </c>
@@ -2604,7 +2636,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>43778</v>
       </c>
@@ -2621,7 +2653,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>43778</v>
       </c>
@@ -2638,7 +2670,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>43784</v>
       </c>
@@ -2655,7 +2687,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>43784</v>
       </c>
@@ -2692,7 +2724,7 @@
         <v>179</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -2715,7 +2747,7 @@
         <v>183</v>
       </c>
       <c r="G90" s="4" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -2761,10 +2793,10 @@
         <v>174</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>43785</v>
       </c>
@@ -2824,7 +2856,7 @@
         <v>180</v>
       </c>
       <c r="G95" s="4" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -2850,7 +2882,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>43789</v>
       </c>
@@ -2867,7 +2899,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>43789</v>
       </c>
@@ -2884,7 +2916,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>43790</v>
       </c>
@@ -2901,7 +2933,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>43790</v>
       </c>
@@ -2941,7 +2973,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>43792</v>
       </c>
@@ -2958,7 +2990,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>43792</v>
       </c>
@@ -2998,7 +3030,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>43796</v>
       </c>
@@ -3015,7 +3047,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>43796</v>
       </c>
@@ -3032,7 +3064,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>43798</v>
       </c>
@@ -3092,7 +3124,7 @@
         <v>183</v>
       </c>
       <c r="G109" s="4" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -3138,7 +3170,7 @@
         <v>175</v>
       </c>
       <c r="G111" s="4" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -3184,10 +3216,10 @@
         <v>177</v>
       </c>
       <c r="G113" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>43799</v>
       </c>
@@ -3204,7 +3236,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>43799</v>
       </c>
@@ -3244,7 +3276,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>43803</v>
       </c>
@@ -3261,7 +3293,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>43803</v>
       </c>
@@ -3301,7 +3333,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>43805</v>
       </c>
@@ -3318,7 +3350,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>43805</v>
       </c>
@@ -3335,7 +3367,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>43805</v>
       </c>
@@ -3352,7 +3384,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>43805</v>
       </c>
@@ -3369,7 +3401,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>43810</v>
       </c>
@@ -3386,7 +3418,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>43810</v>
       </c>
@@ -3403,7 +3435,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>43812</v>
       </c>
@@ -3463,10 +3495,10 @@
         <v>184</v>
       </c>
       <c r="G128" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>43812</v>
       </c>
@@ -3483,7 +3515,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>43813</v>
       </c>
@@ -3500,7 +3532,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>43813</v>
       </c>
@@ -3517,7 +3549,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>43813</v>
       </c>
@@ -3557,7 +3589,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>43813</v>
       </c>
@@ -3574,7 +3606,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>43813</v>
       </c>
@@ -3591,7 +3623,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>43817</v>
       </c>
@@ -3608,7 +3640,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>43817</v>
       </c>
@@ -3625,7 +3657,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>43819</v>
       </c>
@@ -3642,7 +3674,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>43839</v>
       </c>
@@ -3659,7 +3691,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>43839</v>
       </c>
@@ -3676,7 +3708,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>43839</v>
       </c>
@@ -3693,7 +3725,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>43839</v>
       </c>
@@ -3773,7 +3805,7 @@
       </c>
       <c r="G145" s="4"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>43840</v>
       </c>
@@ -3811,7 +3843,7 @@
       </c>
       <c r="G147" s="4"/>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>43841</v>
       </c>
@@ -3828,7 +3860,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>43846</v>
       </c>
@@ -3887,7 +3919,7 @@
       </c>
       <c r="G151" s="4"/>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>43848</v>
       </c>
@@ -3904,7 +3936,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>43848</v>
       </c>
@@ -3921,7 +3953,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>43848</v>
       </c>
@@ -3959,7 +3991,7 @@
       </c>
       <c r="G155" s="4"/>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>43850</v>
       </c>
@@ -3976,7 +4008,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>43851</v>
       </c>
@@ -4035,7 +4067,7 @@
       </c>
       <c r="G159" s="4"/>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>43854</v>
       </c>
@@ -4094,7 +4126,7 @@
       </c>
       <c r="G162" s="4"/>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>43861</v>
       </c>
@@ -4153,7 +4185,7 @@
       </c>
       <c r="G165" s="4"/>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>43861</v>
       </c>
@@ -4170,7 +4202,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>43861</v>
       </c>
@@ -4187,7 +4219,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>43862</v>
       </c>
@@ -4225,7 +4257,7 @@
       </c>
       <c r="G169" s="4"/>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>43866</v>
       </c>
@@ -4242,7 +4274,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>43866</v>
       </c>
@@ -4259,7 +4291,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>43866</v>
       </c>
@@ -4276,7 +4308,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>43866</v>
       </c>
@@ -4335,7 +4367,7 @@
       </c>
       <c r="G175" s="4"/>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>43868</v>
       </c>
@@ -4352,7 +4384,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>43868</v>
       </c>
@@ -4390,7 +4422,7 @@
       </c>
       <c r="G178" s="4"/>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>43868</v>
       </c>
@@ -4428,7 +4460,7 @@
       </c>
       <c r="G180" s="4"/>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>43876</v>
       </c>
@@ -4508,7 +4540,7 @@
       </c>
       <c r="G184" s="4"/>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>43896</v>
       </c>
@@ -4525,7 +4557,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>43896</v>
       </c>
@@ -4542,7 +4574,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>43896</v>
       </c>
@@ -4559,7 +4591,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>43897</v>
       </c>
@@ -4593,11 +4625,11 @@
         <v>10</v>
       </c>
       <c r="F189" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G189" s="4"/>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>43902</v>
       </c>
@@ -4614,7 +4646,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>43902</v>
       </c>
@@ -4652,7 +4684,7 @@
       </c>
       <c r="G192" s="4"/>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>43903</v>
       </c>
@@ -4711,7 +4743,7 @@
       </c>
       <c r="G195" s="4"/>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>43908</v>
       </c>
@@ -4728,7 +4760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>43908</v>
       </c>
@@ -4762,7 +4794,7 @@
         <v>10</v>
       </c>
       <c r="F198" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G198" s="4"/>
     </row>
@@ -4787,7 +4819,7 @@
       </c>
       <c r="G199" s="4"/>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>43910</v>
       </c>
@@ -4804,7 +4836,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>43911</v>
       </c>
@@ -4821,7 +4853,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>43911</v>
       </c>
@@ -4838,7 +4870,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>43911</v>
       </c>
@@ -4855,7 +4887,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>43915</v>
       </c>
@@ -4872,7 +4904,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>43915</v>
       </c>
@@ -4889,7 +4921,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>43915</v>
       </c>
@@ -4906,7 +4938,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>43915</v>
       </c>
@@ -5028,7 +5060,7 @@
       </c>
       <c r="G212" s="4"/>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>43917</v>
       </c>
@@ -5045,7 +5077,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>43918</v>
       </c>
@@ -5100,7 +5132,7 @@
         <v>16</v>
       </c>
       <c r="F216" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G216" s="4"/>
     </row>
@@ -5125,7 +5157,7 @@
       </c>
       <c r="G217" s="4"/>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>43924</v>
       </c>
@@ -5163,7 +5195,7 @@
       </c>
       <c r="G219" s="4"/>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>43924</v>
       </c>
@@ -5180,7 +5212,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>43925</v>
       </c>
@@ -5197,7 +5229,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>43929</v>
       </c>
@@ -5214,7 +5246,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>43930</v>
       </c>
@@ -5231,7 +5263,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>43930</v>
       </c>
@@ -5248,7 +5280,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>43937</v>
       </c>
@@ -5265,7 +5297,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>43937</v>
       </c>
@@ -5282,7 +5314,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>43938</v>
       </c>
@@ -5316,7 +5348,7 @@
         <v>10</v>
       </c>
       <c r="F228" s="4" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="G228" s="4"/>
     </row>
@@ -5341,7 +5373,7 @@
       </c>
       <c r="G229" s="4"/>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>43938</v>
       </c>
@@ -5358,7 +5390,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>43939</v>
       </c>
@@ -5375,7 +5407,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>43939</v>
       </c>
@@ -5413,9 +5445,142 @@
       </c>
       <c r="G233" s="4"/>
     </row>
+    <row r="241" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E241" t="s">
+        <v>185</v>
+      </c>
+      <c r="F241">
+        <f>COUNTIF(F1:F234, "Alouis*")</f>
+        <v>10</v>
+      </c>
+      <c r="G241">
+        <f>COUNTIF(G1:G234, "Alouis*")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E242" t="s">
+        <v>182</v>
+      </c>
+      <c r="F242">
+        <f>COUNTIF(F1:F234, "D1")</f>
+        <v>8</v>
+      </c>
+      <c r="G242">
+        <f>COUNTIF(G2:G235, "D1")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="243" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E243" t="s">
+        <v>174</v>
+      </c>
+      <c r="F243">
+        <f>COUNTIF(F2:F235, "D2")</f>
+        <v>8</v>
+      </c>
+      <c r="G243">
+        <f>COUNTIF(G2:G234, "D2")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="244" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E244" t="s">
+        <v>173</v>
+      </c>
+      <c r="F244">
+        <f>COUNTIF(F2:F235, "D3")</f>
+        <v>8</v>
+      </c>
+      <c r="G244">
+        <f>COUNTIF(G2:G234, "D3")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="245" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E245" t="s">
+        <v>179</v>
+      </c>
+      <c r="F245">
+        <f>COUNTIF(F2:F234, "D4")</f>
+        <v>8</v>
+      </c>
+      <c r="G245">
+        <f>COUNTIF(G2:G234, "D4")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="246" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E246" t="s">
+        <v>176</v>
+      </c>
+      <c r="F246">
+        <f>COUNTIF(F5:F238, "D1")</f>
+        <v>8</v>
+      </c>
+      <c r="G246">
+        <f>COUNTIF(G2:G234, "D5")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="247" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E247" t="s">
+        <v>177</v>
+      </c>
+      <c r="F247">
+        <f>COUNTIF(F2:F234, "H1")</f>
+        <v>8</v>
+      </c>
+      <c r="G247">
+        <f>COUNTIF(G2:G234, "H1")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="248" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E248" t="s">
+        <v>181</v>
+      </c>
+      <c r="F248">
+        <f>COUNTIF(F2:F234, "H2")</f>
+        <v>8</v>
+      </c>
+      <c r="G248">
+        <f>COUNTIF(G2:G234, "H2")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="249" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E249" t="s">
+        <v>186</v>
+      </c>
+      <c r="F249">
+        <f>COUNTIF(F2:F234, "Henk*")</f>
+        <v>13</v>
+      </c>
+      <c r="G249">
+        <f t="shared" ref="G242:G249" si="0">COUNTIF(G9:G242, "Alouis*")</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <autoFilter ref="A1:G233" xr:uid="{47F88E0C-9F17-4727-BABF-EEEB9EA2FD37}"/>
+  <autoFilter ref="A1:G233" xr:uid="{47F88E0C-9F17-4727-BABF-EEEB9EA2FD37}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Volley '68 DS 1"/>
+        <filter val="Volley '68 DS 2"/>
+        <filter val="Volley '68 DS 3"/>
+        <filter val="Volley '68 DS 4"/>
+        <filter val="Volley '68 DS 5"/>
+        <filter val="Volley '68 HS 1"/>
+        <filter val="Volley '68 HS 2"/>
+        <filter val="Volley '68 JC 1"/>
+        <filter val="Volley '68 MA 1"/>
+        <filter val="Volley '68 MA 2"/>
+        <filter val="Volley '68 MC 1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
binary wijzigingen worden niet gepushed?
</commit_message>
<xml_diff>
--- a/Thuiswedstrijden.xlsx
+++ b/Thuiswedstrijden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\github\volleybalwedstrijdschema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04526884-9292-47FB-B3DE-84D852E4661D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1E4326-8EA6-4365-A8E7-1060212BC338}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -624,7 +624,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -643,8 +643,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -654,6 +661,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -666,11 +678,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -678,8 +691,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -986,8 +1001,8 @@
   <dimension ref="A1:G249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E255" sqref="E255"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,7 +1536,7 @@
       <c r="E27" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="7" t="s">
         <v>193</v>
       </c>
       <c r="G27" s="4" t="s">
@@ -1828,7 +1843,7 @@
       <c r="E44" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F44" s="7" t="s">
         <v>193</v>
       </c>
       <c r="G44" s="4" t="s">
@@ -2080,7 +2095,7 @@
       <c r="E56" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F56" s="4" t="s">
+      <c r="F56" s="7" t="s">
         <v>193</v>
       </c>
       <c r="G56" s="4" t="s">
@@ -2725,7 +2740,7 @@
       <c r="E89" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F89" s="4" t="s">
+      <c r="F89" s="7" t="s">
         <v>193</v>
       </c>
       <c r="G89" s="4" t="s">
@@ -3473,7 +3488,7 @@
       <c r="E127" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F127" s="4" t="s">
+      <c r="F127" s="7" t="s">
         <v>193</v>
       </c>
       <c r="G127" s="4" t="s">

</xml_diff>